<commit_message>
last function in helper
</commit_message>
<xml_diff>
--- a/outputs/tables/reduced_llm_per_video.xlsx
+++ b/outputs/tables/reduced_llm_per_video.xlsx
@@ -34,15 +34,15 @@
     <t>gpt-5.1 [T0.5-With-K]</t>
   </si>
   <si>
+    <t>gpt-5.1 [T0.5-No-K]</t>
+  </si>
+  <si>
+    <t>moonshotai_Kimi-K2-Thinking [T0.5-With-K]</t>
+  </si>
+  <si>
     <t>gemini-2.5-flash [T0.5-No-K]</t>
   </si>
   <si>
-    <t>gpt-5.1 [T0.5-No-K]</t>
-  </si>
-  <si>
-    <t>moonshotai_Kimi-K2-Thinking [T0.5-With-K]</t>
-  </si>
-  <si>
     <t>gemini-2.5-flash [T0-With-K]</t>
   </si>
   <si>
@@ -148,349 +148,349 @@
     <t>openai_gpt-oss-20b [T0-With-K]</t>
   </si>
   <si>
-    <t>0.650 / 0.730</t>
-  </si>
-  <si>
-    <t>0.663 (0.650 - 0.670) / 0.760 (0.750 - 0.770)</t>
-  </si>
-  <si>
-    <t>0.637 (0.590 - 0.670) / 0.707 (0.690 - 0.720)</t>
-  </si>
-  <si>
-    <t>0.630 (0.600 - 0.650) / 0.733 (0.700 - 0.770)</t>
-  </si>
-  <si>
-    <t>0.583 (0.520 - 0.640) / 0.680 (0.610 - 0.730)</t>
-  </si>
-  <si>
-    <t>0.470 / 0.590</t>
-  </si>
-  <si>
-    <t>0.600 (0.570 - 0.640) / 0.690 (0.680 - 0.710)</t>
-  </si>
-  <si>
-    <t>0.600 / 0.700</t>
-  </si>
-  <si>
-    <t>0.617 (0.590 - 0.640) / 0.717 (0.710 - 0.730)</t>
-  </si>
-  <si>
-    <t>0.620 / 0.720</t>
-  </si>
-  <si>
-    <t>0.460 / 0.570</t>
-  </si>
-  <si>
-    <t>0.640 / 0.730</t>
-  </si>
-  <si>
-    <t>0.630 / 0.690</t>
-  </si>
-  <si>
-    <t>0.533 (0.530 - 0.540) / 0.667 (0.660 - 0.670)</t>
-  </si>
-  <si>
-    <t>0.547 (0.480 - 0.630) / 0.607 (0.520 - 0.700)</t>
-  </si>
-  <si>
-    <t>0.567 (0.530 - 0.590) / 0.673 (0.650 - 0.690)</t>
-  </si>
-  <si>
-    <t>0.603 (0.580 - 0.620) / 0.667 (0.650 - 0.680)</t>
-  </si>
-  <si>
-    <t>0.460 (0.440 - 0.480) / 0.553 (0.520 - 0.580)</t>
-  </si>
-  <si>
-    <t>0.580 / 0.670</t>
-  </si>
-  <si>
-    <t>0.510 / 0.620</t>
-  </si>
-  <si>
-    <t>0.560 / 0.670</t>
-  </si>
-  <si>
-    <t>0.700 / 0.750</t>
-  </si>
-  <si>
-    <t>0.470 / 0.570</t>
-  </si>
-  <si>
-    <t>0.467 (0.370 - 0.530) / 0.527 (0.430 - 0.600)</t>
-  </si>
-  <si>
-    <t>0.580 (0.580 - 0.580) / 0.663 (0.660 - 0.670)</t>
-  </si>
-  <si>
-    <t>0.660 / 0.700</t>
-  </si>
-  <si>
-    <t>0.643 (0.600 - 0.710) / 0.707 (0.670 - 0.740)</t>
-  </si>
-  <si>
-    <t>0.433 (0.210 - 0.560) / 0.517 (0.290 - 0.650)</t>
-  </si>
-  <si>
-    <t>0.500 / 0.620</t>
-  </si>
-  <si>
-    <t>0.450 / 0.550</t>
-  </si>
-  <si>
-    <t>0.210 / 0.280</t>
-  </si>
-  <si>
-    <t>0.543 (0.490 - 0.570) / 0.667 (0.620 - 0.690)</t>
-  </si>
-  <si>
-    <t>0.590 (0.550 - 0.620) / 0.650 (0.620 - 0.670)</t>
-  </si>
-  <si>
-    <t>0.387 (0.320 - 0.420) / 0.477 (0.420 - 0.520)</t>
-  </si>
-  <si>
-    <t>0.603 (0.590 - 0.610) / 0.707 (0.700 - 0.710)</t>
-  </si>
-  <si>
-    <t>0.517 (0.490 - 0.560) / 0.569 (0.520 - 0.610)</t>
-  </si>
-  <si>
-    <t>0.460 / 0.520</t>
-  </si>
-  <si>
-    <t>0.380 / 0.430</t>
-  </si>
-  <si>
-    <t>0.760 / 0.820</t>
-  </si>
-  <si>
-    <t>0.723 (0.700 - 0.760) / 0.783 (0.750 - 0.830)</t>
-  </si>
-  <si>
-    <t>0.613 (0.350 - 0.770) / 0.720 (0.450 - 0.880)</t>
-  </si>
-  <si>
-    <t>0.700 (0.520 - 0.830) / 0.763 (0.590 - 0.870)</t>
-  </si>
-  <si>
-    <t>0.630 (0.570 - 0.700) / 0.737 (0.670 - 0.800)</t>
-  </si>
-  <si>
-    <t>0.650 / 0.740</t>
-  </si>
-  <si>
-    <t>0.773 (0.760 - 0.780) / 0.857 (0.830 - 0.870)</t>
-  </si>
-  <si>
-    <t>0.770 / 0.850</t>
-  </si>
-  <si>
-    <t>0.817 (0.810 - 0.830) / 0.867 (0.860 - 0.870)</t>
-  </si>
-  <si>
-    <t>0.830 / 0.870</t>
-  </si>
-  <si>
-    <t>0.640 / 0.740</t>
-  </si>
-  <si>
-    <t>0.790 / 0.860</t>
-  </si>
-  <si>
-    <t>0.790 / 0.870</t>
-  </si>
-  <si>
-    <t>0.720 / 0.830</t>
-  </si>
-  <si>
-    <t>0.640 (0.600 - 0.670) / 0.723 (0.680 - 0.750)</t>
-  </si>
-  <si>
-    <t>0.407 (0.230 - 0.750) / 0.503 (0.320 - 0.840)</t>
-  </si>
-  <si>
-    <t>0.613 (0.590 - 0.640) / 0.703 (0.680 - 0.730)</t>
-  </si>
-  <si>
-    <t>0.733 (0.720 - 0.740) / 0.833 (0.830 - 0.840)</t>
-  </si>
-  <si>
-    <t>0.463 (0.440 - 0.500) / 0.583 (0.560 - 0.610)</t>
-  </si>
-  <si>
-    <t>0.750 / 0.850</t>
-  </si>
-  <si>
-    <t>0.650 / 0.750</t>
-  </si>
-  <si>
-    <t>0.720 / 0.840</t>
-  </si>
-  <si>
-    <t>0.730 / 0.820</t>
-  </si>
-  <si>
-    <t>0.460 / 0.560</t>
-  </si>
-  <si>
-    <t>0.460 / 0.580</t>
-  </si>
-  <si>
-    <t>0.427 (0.360 - 0.500) / 0.523 (0.480 - 0.590)</t>
-  </si>
-  <si>
-    <t>0.743 (0.740 - 0.750) / 0.837 (0.820 - 0.850)</t>
-  </si>
-  <si>
-    <t>0.700 / 0.820</t>
-  </si>
-  <si>
-    <t>0.567 (0.160 - 0.780) / 0.653 (0.250 - 0.870)</t>
-  </si>
-  <si>
-    <t>0.153 (0.140 - 0.160) / 0.247 (0.230 - 0.270)</t>
-  </si>
-  <si>
-    <t>0.710 / 0.770</t>
-  </si>
-  <si>
-    <t>0.350 / 0.430</t>
-  </si>
-  <si>
-    <t>0.380 / 0.460</t>
-  </si>
-  <si>
-    <t>0.633 (0.610 - 0.670) / 0.707 (0.680 - 0.750)</t>
-  </si>
-  <si>
-    <t>0.713 (0.690 - 0.730) / 0.823 (0.810 - 0.830)</t>
-  </si>
-  <si>
-    <t>0.447 (0.410 - 0.500) / 0.540 (0.490 - 0.600)</t>
-  </si>
-  <si>
-    <t>0.733 (0.720 - 0.750) / 0.820 (0.810 - 0.830)</t>
-  </si>
-  <si>
-    <t>0.500 (0.430 - 0.540) / 0.613 (0.540 - 0.660)</t>
-  </si>
-  <si>
-    <t>0.470 / 0.600</t>
-  </si>
-  <si>
-    <t>0.200 / 0.270</t>
-  </si>
-  <si>
-    <t>0.590 / 0.650</t>
-  </si>
-  <si>
-    <t>0.533 (0.490 - 0.590) / 0.597 (0.550 - 0.660)</t>
-  </si>
-  <si>
-    <t>0.480 (0.450 - 0.500) / 0.547 (0.510 - 0.570)</t>
-  </si>
-  <si>
-    <t>0.477 (0.470 - 0.480) / 0.573 (0.560 - 0.590)</t>
-  </si>
-  <si>
-    <t>0.477 (0.460 - 0.490) / 0.583 (0.560 - 0.610)</t>
-  </si>
-  <si>
-    <t>0.470 / 0.550</t>
-  </si>
-  <si>
-    <t>0.467 (0.410 - 0.520) / 0.543 (0.500 - 0.580)</t>
-  </si>
-  <si>
-    <t>0.460 / 0.550</t>
-  </si>
-  <si>
-    <t>0.457 (0.440 - 0.470) / 0.563 (0.550 - 0.580)</t>
-  </si>
-  <si>
-    <t>0.450 / 0.560</t>
-  </si>
-  <si>
-    <t>0.430 / 0.530</t>
-  </si>
-  <si>
-    <t>0.430 / 0.510</t>
-  </si>
-  <si>
-    <t>0.420 / 0.490</t>
-  </si>
-  <si>
-    <t>0.413 (0.400 - 0.440) / 0.517 (0.500 - 0.530)</t>
-  </si>
-  <si>
-    <t>0.410 (0.310 - 0.470) / 0.500 (0.410 - 0.550)</t>
-  </si>
-  <si>
-    <t>0.403 (0.400 - 0.410) / 0.513 (0.510 - 0.520)</t>
-  </si>
-  <si>
-    <t>0.400 (0.370 - 0.450) / 0.470 (0.440 - 0.500)</t>
-  </si>
-  <si>
-    <t>0.400 (0.370 - 0.430) / 0.470 (0.450 - 0.490)</t>
-  </si>
-  <si>
-    <t>0.390 / 0.530</t>
-  </si>
-  <si>
-    <t>0.390 / 0.500</t>
-  </si>
-  <si>
-    <t>0.390 / 0.490</t>
-  </si>
-  <si>
-    <t>0.380 / 0.480</t>
-  </si>
-  <si>
-    <t>0.380 / 0.470</t>
-  </si>
-  <si>
-    <t>0.357 (0.330 - 0.380) / 0.440 (0.410 - 0.480)</t>
-  </si>
-  <si>
-    <t>0.357 (0.320 - 0.390) / 0.473 (0.430 - 0.520)</t>
-  </si>
-  <si>
-    <t>0.350 / 0.420</t>
-  </si>
-  <si>
-    <t>0.343 (0.270 - 0.420) / 0.443 (0.400 - 0.510)</t>
-  </si>
-  <si>
-    <t>0.323 (0.290 - 0.360) / 0.397 (0.340 - 0.430)</t>
-  </si>
-  <si>
-    <t>0.310 / 0.430</t>
-  </si>
-  <si>
-    <t>0.310 / 0.410</t>
-  </si>
-  <si>
-    <t>0.310 / 0.350</t>
-  </si>
-  <si>
-    <t>0.300 (0.290 - 0.320) / 0.423 (0.410 - 0.450)</t>
-  </si>
-  <si>
-    <t>0.293 (0.280 - 0.310) / 0.353 (0.340 - 0.360)</t>
-  </si>
-  <si>
-    <t>0.283 (0.260 - 0.310) / 0.377 (0.370 - 0.380)</t>
-  </si>
-  <si>
-    <t>0.283 (0.250 - 0.340) / 0.400 (0.370 - 0.450)</t>
-  </si>
-  <si>
-    <t>0.237 (0.230 - 0.250) / 0.313 (0.300 - 0.320)</t>
-  </si>
-  <si>
-    <t>0.210 / 0.300</t>
+    <t>0.65 / 0.73</t>
+  </si>
+  <si>
+    <t>0.66 (0.65 - 0.67) / 0.76 (0.75 - 0.77)</t>
+  </si>
+  <si>
+    <t>0.63 (0.60 - 0.65) / 0.73 (0.70 - 0.77)</t>
+  </si>
+  <si>
+    <t>0.58 (0.52 - 0.64) / 0.68 (0.61 - 0.73)</t>
+  </si>
+  <si>
+    <t>0.64 (0.59 - 0.67) / 0.71 (0.69 - 0.72)</t>
+  </si>
+  <si>
+    <t>0.47 / 0.59</t>
+  </si>
+  <si>
+    <t>0.60 (0.57 - 0.64) / 0.69 (0.68 - 0.71)</t>
+  </si>
+  <si>
+    <t>0.60 / 0.70</t>
+  </si>
+  <si>
+    <t>0.62 (0.59 - 0.64) / 0.72 (0.71 - 0.73)</t>
+  </si>
+  <si>
+    <t>0.62 / 0.72</t>
+  </si>
+  <si>
+    <t>0.46 / 0.57</t>
+  </si>
+  <si>
+    <t>0.64 / 0.73</t>
+  </si>
+  <si>
+    <t>0.63 / 0.69</t>
+  </si>
+  <si>
+    <t>0.53 (0.53 - 0.54) / 0.67 (0.66 - 0.67)</t>
+  </si>
+  <si>
+    <t>0.55 (0.48 - 0.63) / 0.61 (0.52 - 0.70)</t>
+  </si>
+  <si>
+    <t>0.57 (0.53 - 0.59) / 0.67 (0.65 - 0.69)</t>
+  </si>
+  <si>
+    <t>0.60 (0.58 - 0.62) / 0.67 (0.65 - 0.68)</t>
+  </si>
+  <si>
+    <t>0.46 (0.44 - 0.48) / 0.55 (0.52 - 0.58)</t>
+  </si>
+  <si>
+    <t>0.58 / 0.67</t>
+  </si>
+  <si>
+    <t>0.51 / 0.62</t>
+  </si>
+  <si>
+    <t>0.56 / 0.67</t>
+  </si>
+  <si>
+    <t>0.70 / 0.75</t>
+  </si>
+  <si>
+    <t>0.47 / 0.57</t>
+  </si>
+  <si>
+    <t>0.47 (0.37 - 0.53) / 0.53 (0.43 - 0.60)</t>
+  </si>
+  <si>
+    <t>0.58 (0.58 - 0.58) / 0.66 (0.66 - 0.67)</t>
+  </si>
+  <si>
+    <t>0.66 / 0.70</t>
+  </si>
+  <si>
+    <t>0.64 (0.60 - 0.71) / 0.71 (0.67 - 0.74)</t>
+  </si>
+  <si>
+    <t>0.43 (0.21 - 0.56) / 0.52 (0.29 - 0.65)</t>
+  </si>
+  <si>
+    <t>0.50 / 0.62</t>
+  </si>
+  <si>
+    <t>0.45 / 0.55</t>
+  </si>
+  <si>
+    <t>0.21 / 0.28</t>
+  </si>
+  <si>
+    <t>0.54 (0.49 - 0.57) / 0.67 (0.62 - 0.69)</t>
+  </si>
+  <si>
+    <t>0.59 (0.55 - 0.62) / 0.65 (0.62 - 0.67)</t>
+  </si>
+  <si>
+    <t>0.39 (0.32 - 0.42) / 0.48 (0.42 - 0.52)</t>
+  </si>
+  <si>
+    <t>0.60 (0.59 - 0.61) / 0.71 (0.70 - 0.71)</t>
+  </si>
+  <si>
+    <t>0.52 (0.49 - 0.56) / 0.57 (0.52 - 0.61)</t>
+  </si>
+  <si>
+    <t>0.46 / 0.52</t>
+  </si>
+  <si>
+    <t>0.38 / 0.43</t>
+  </si>
+  <si>
+    <t>0.76 / 0.82</t>
+  </si>
+  <si>
+    <t>0.72 (0.70 - 0.76) / 0.78 (0.75 - 0.83)</t>
+  </si>
+  <si>
+    <t>0.70 (0.52 - 0.83) / 0.76 (0.59 - 0.87)</t>
+  </si>
+  <si>
+    <t>0.63 (0.57 - 0.70) / 0.74 (0.67 - 0.80)</t>
+  </si>
+  <si>
+    <t>0.61 (0.35 - 0.77) / 0.72 (0.45 - 0.88)</t>
+  </si>
+  <si>
+    <t>0.65 / 0.74</t>
+  </si>
+  <si>
+    <t>0.77 (0.76 - 0.78) / 0.86 (0.83 - 0.87)</t>
+  </si>
+  <si>
+    <t>0.77 / 0.85</t>
+  </si>
+  <si>
+    <t>0.82 (0.81 - 0.83) / 0.87 (0.86 - 0.87)</t>
+  </si>
+  <si>
+    <t>0.83 / 0.87</t>
+  </si>
+  <si>
+    <t>0.64 / 0.74</t>
+  </si>
+  <si>
+    <t>0.79 / 0.86</t>
+  </si>
+  <si>
+    <t>0.79 / 0.87</t>
+  </si>
+  <si>
+    <t>0.72 / 0.83</t>
+  </si>
+  <si>
+    <t>0.64 (0.60 - 0.67) / 0.72 (0.68 - 0.75)</t>
+  </si>
+  <si>
+    <t>0.41 (0.23 - 0.75) / 0.50 (0.32 - 0.84)</t>
+  </si>
+  <si>
+    <t>0.61 (0.59 - 0.64) / 0.70 (0.68 - 0.73)</t>
+  </si>
+  <si>
+    <t>0.73 (0.72 - 0.74) / 0.83 (0.83 - 0.84)</t>
+  </si>
+  <si>
+    <t>0.46 (0.44 - 0.50) / 0.58 (0.56 - 0.61)</t>
+  </si>
+  <si>
+    <t>0.75 / 0.85</t>
+  </si>
+  <si>
+    <t>0.65 / 0.75</t>
+  </si>
+  <si>
+    <t>0.72 / 0.84</t>
+  </si>
+  <si>
+    <t>0.73 / 0.82</t>
+  </si>
+  <si>
+    <t>0.46 / 0.56</t>
+  </si>
+  <si>
+    <t>0.46 / 0.58</t>
+  </si>
+  <si>
+    <t>0.43 (0.36 - 0.50) / 0.52 (0.48 - 0.59)</t>
+  </si>
+  <si>
+    <t>0.74 (0.74 - 0.75) / 0.84 (0.82 - 0.85)</t>
+  </si>
+  <si>
+    <t>0.70 / 0.82</t>
+  </si>
+  <si>
+    <t>0.57 (0.16 - 0.78) / 0.65 (0.25 - 0.87)</t>
+  </si>
+  <si>
+    <t>0.15 (0.14 - 0.16) / 0.25 (0.23 - 0.27)</t>
+  </si>
+  <si>
+    <t>0.71 / 0.77</t>
+  </si>
+  <si>
+    <t>0.35 / 0.43</t>
+  </si>
+  <si>
+    <t>0.38 / 0.46</t>
+  </si>
+  <si>
+    <t>0.63 (0.61 - 0.67) / 0.71 (0.68 - 0.75)</t>
+  </si>
+  <si>
+    <t>0.71 (0.69 - 0.73) / 0.82 (0.81 - 0.83)</t>
+  </si>
+  <si>
+    <t>0.45 (0.41 - 0.50) / 0.54 (0.49 - 0.60)</t>
+  </si>
+  <si>
+    <t>0.73 (0.72 - 0.75) / 0.82 (0.81 - 0.83)</t>
+  </si>
+  <si>
+    <t>0.50 (0.43 - 0.54) / 0.61 (0.54 - 0.66)</t>
+  </si>
+  <si>
+    <t>0.47 / 0.60</t>
+  </si>
+  <si>
+    <t>0.20 / 0.27</t>
+  </si>
+  <si>
+    <t>0.59 / 0.65</t>
+  </si>
+  <si>
+    <t>0.53 (0.49 - 0.59) / 0.60 (0.55 - 0.66)</t>
+  </si>
+  <si>
+    <t>0.48 (0.47 - 0.48) / 0.57 (0.56 - 0.59)</t>
+  </si>
+  <si>
+    <t>0.48 (0.46 - 0.49) / 0.58 (0.56 - 0.61)</t>
+  </si>
+  <si>
+    <t>0.48 (0.45 - 0.50) / 0.55 (0.51 - 0.57)</t>
+  </si>
+  <si>
+    <t>0.47 / 0.55</t>
+  </si>
+  <si>
+    <t>0.47 (0.41 - 0.52) / 0.54 (0.50 - 0.58)</t>
+  </si>
+  <si>
+    <t>0.46 / 0.55</t>
+  </si>
+  <si>
+    <t>0.46 (0.44 - 0.47) / 0.56 (0.55 - 0.58)</t>
+  </si>
+  <si>
+    <t>0.45 / 0.56</t>
+  </si>
+  <si>
+    <t>0.43 / 0.53</t>
+  </si>
+  <si>
+    <t>0.43 / 0.51</t>
+  </si>
+  <si>
+    <t>0.42 / 0.49</t>
+  </si>
+  <si>
+    <t>0.41 (0.40 - 0.44) / 0.52 (0.50 - 0.53)</t>
+  </si>
+  <si>
+    <t>0.41 (0.31 - 0.47) / 0.50 (0.41 - 0.55)</t>
+  </si>
+  <si>
+    <t>0.40 (0.40 - 0.41) / 0.51 (0.51 - 0.52)</t>
+  </si>
+  <si>
+    <t>0.40 (0.37 - 0.45) / 0.47 (0.44 - 0.50)</t>
+  </si>
+  <si>
+    <t>0.40 (0.37 - 0.43) / 0.47 (0.45 - 0.49)</t>
+  </si>
+  <si>
+    <t>0.39 / 0.53</t>
+  </si>
+  <si>
+    <t>0.39 / 0.50</t>
+  </si>
+  <si>
+    <t>0.39 / 0.49</t>
+  </si>
+  <si>
+    <t>0.38 / 0.48</t>
+  </si>
+  <si>
+    <t>0.38 / 0.47</t>
+  </si>
+  <si>
+    <t>0.36 (0.33 - 0.38) / 0.44 (0.41 - 0.48)</t>
+  </si>
+  <si>
+    <t>0.36 (0.32 - 0.39) / 0.47 (0.43 - 0.52)</t>
+  </si>
+  <si>
+    <t>0.35 / 0.42</t>
+  </si>
+  <si>
+    <t>0.34 (0.27 - 0.42) / 0.44 (0.40 - 0.51)</t>
+  </si>
+  <si>
+    <t>0.32 (0.29 - 0.36) / 0.40 (0.34 - 0.43)</t>
+  </si>
+  <si>
+    <t>0.31 / 0.43</t>
+  </si>
+  <si>
+    <t>0.31 / 0.41</t>
+  </si>
+  <si>
+    <t>0.31 / 0.35</t>
+  </si>
+  <si>
+    <t>0.30 (0.29 - 0.32) / 0.42 (0.41 - 0.45)</t>
+  </si>
+  <si>
+    <t>0.29 (0.28 - 0.31) / 0.35 (0.34 - 0.36)</t>
+  </si>
+  <si>
+    <t>0.28 (0.26 - 0.31) / 0.38 (0.37 - 0.38)</t>
+  </si>
+  <si>
+    <t>0.28 (0.25 - 0.34) / 0.40 (0.37 - 0.45)</t>
+  </si>
+  <si>
+    <t>0.24 (0.23 - 0.25) / 0.31 (0.30 - 0.32)</t>
+  </si>
+  <si>
+    <t>0.21 / 0.30</t>
   </si>
 </sst>
 </file>

</xml_diff>